<commit_message>
Tree Editor now supports adding equipment nodes
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>Complete Report</t>
+  </si>
+  <si>
+    <t>Change Attribute to Patient attribute in the Tree editor</t>
+  </si>
+  <si>
+    <t>Handle when equipment node is first node to be inserted</t>
+  </si>
+  <si>
+    <t>Fix bug where when you delete a solution node, you can then insert a patient/equipment attribute node afterwards</t>
+  </si>
+  <si>
+    <t>Change length of numeric attribute to be smaller</t>
   </si>
 </sst>
 </file>
@@ -591,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,6 +959,42 @@
       <c r="B38" s="5"/>
       <c r="C38" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented iteration through trees with equipment nodes
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t>Change length of numeric attribute to be smaller</t>
+  </si>
+  <si>
+    <t>Fix view tree so that the canvas is a bit smaller so that it is easier to scroll up to top of screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get rid of "Index" from all of the pages, and look into renaming the default page titles </t>
+  </si>
+  <si>
+    <t>Edit patients details page so that there are no line breaks in patient attribute display names</t>
   </si>
 </sst>
 </file>
@@ -266,12 +275,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -304,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -314,15 +329,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +648,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="6"/>
@@ -639,7 +657,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="6"/>
@@ -648,7 +666,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="7"/>
@@ -657,7 +675,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="5"/>
@@ -666,7 +684,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="6"/>
@@ -675,7 +693,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6"/>
@@ -684,7 +702,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6"/>
@@ -701,7 +719,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6"/>
@@ -710,7 +728,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="7"/>
@@ -719,7 +737,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="6"/>
@@ -728,7 +746,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="5"/>
@@ -737,7 +755,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="5"/>
@@ -746,7 +764,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="5"/>
@@ -764,7 +782,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="7"/>
@@ -773,7 +791,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="7"/>
@@ -809,7 +827,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="6"/>
@@ -863,7 +881,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="5"/>
@@ -890,7 +908,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="5"/>
@@ -935,7 +953,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="7"/>
@@ -980,7 +998,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B41" s="6"/>
@@ -994,6 +1012,33 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Error handling for parsing an incomplete decision tree
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -166,15 +166,9 @@
     <t>Error handling for tree that can't be parsed</t>
   </si>
   <si>
-    <t>include equipment in tree</t>
-  </si>
-  <si>
     <t>Generate printable handling plans</t>
   </si>
   <si>
-    <t>Add loading things for ajax in tree editor</t>
-  </si>
-  <si>
     <t>Make tree so that you can just click enter on a solution and it will overwrite the current one (or something like that)</t>
   </si>
   <si>
@@ -245,6 +239,15 @@
   </si>
   <si>
     <t>Edit patients details page so that there are no line breaks in patient attribute display names</t>
+  </si>
+  <si>
+    <t>Include equipment in tree</t>
+  </si>
+  <si>
+    <t>Add loading gif for ajax in tree editor</t>
+  </si>
+  <si>
+    <t>Find out what browsers are compatible</t>
   </si>
 </sst>
 </file>
@@ -621,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,13 +641,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +656,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -662,7 +665,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,7 +674,7 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,7 +683,7 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,7 +692,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +701,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,7 +710,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +727,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +736,7 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,7 +745,7 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +754,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +763,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,7 +772,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,7 +781,7 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +799,7 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,7 +808,7 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,7 +817,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +826,7 @@
       </c>
       <c r="B21" s="6"/>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,7 +844,7 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -850,7 +853,7 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,187 +862,196 @@
       </c>
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>46</v>
+      <c r="A27" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1075,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Login, logout, register, list users account functionality working
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>Find out what browsers are compatible</t>
+  </si>
+  <si>
+    <t>Improve view pages layout for equipment</t>
+  </si>
+  <si>
+    <t>Add numeric handling for equipment attributes (important for no. of patient handlers)</t>
+  </si>
+  <si>
+    <t>Check anywhere that there is a completeattribute object used in the model that the field variables are valid</t>
   </si>
 </sst>
 </file>
@@ -624,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,6 +1062,30 @@
       <c r="C46" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished authorization and added users link in navbar
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Check anywhere that there is a completeattribute object used in the model that the field variables are valid</t>
+  </si>
+  <si>
+    <t>Add "active" attribute in the bootstrap nav panel</t>
+  </si>
+  <si>
+    <t>Make "Patient Handling System" look better in the nav bar</t>
   </si>
 </sst>
 </file>
@@ -633,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,11 +1087,32 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B49" s="5"/>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delete user functionality complete
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Make "Patient Handling System" look better in the nav bar</t>
+  </si>
+  <si>
+    <t>Rename AttributeController to PatientAttributeController</t>
   </si>
 </sst>
 </file>
@@ -639,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,6 +1114,15 @@
       </c>
       <c r="B51" s="7"/>
       <c r="C51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for inserting videos into solutions
</commit_message>
<xml_diff>
--- a/Documentation/Requirements Progress.xlsx
+++ b/Documentation/Requirements Progress.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t xml:space="preserve">Enable all patient handlers to be able to view all of the handling plans for a particular patient </t>
   </si>
@@ -229,9 +229,6 @@
     <t>Fix bug where when you delete a solution node, you can then insert a patient/equipment attribute node afterwards</t>
   </si>
   <si>
-    <t>Change length of numeric attribute to be smaller</t>
-  </si>
-  <si>
     <t>Fix view tree so that the canvas is a bit smaller so that it is easier to scroll up to top of screen</t>
   </si>
   <si>
@@ -277,7 +274,13 @@
     <t>Fix bug where solution title doesn’t go in when creating decision tree</t>
   </si>
   <si>
-    <t>Fix bug with weight</t>
+    <t>Fix bug with weight, i.e. make that attribute non editable</t>
+  </si>
+  <si>
+    <t>Add support for adding images</t>
+  </si>
+  <si>
+    <t>Change length of numeric attribute form box to be smaller</t>
   </si>
 </sst>
 </file>
@@ -654,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,12 +845,12 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +909,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
@@ -924,7 +927,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" t="s">
@@ -1004,12 +1007,12 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1044,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" t="s">
@@ -1050,7 +1053,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" t="s">
@@ -1058,17 +1061,17 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>69</v>
+      <c r="A44" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" t="s">
@@ -1077,16 +1080,16 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" t="s">
@@ -1095,7 +1098,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" t="s">
@@ -1104,7 +1107,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" t="s">
@@ -1113,7 +1116,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" t="s">
@@ -1122,7 +1125,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" t="s">
@@ -1131,7 +1134,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" t="s">
@@ -1139,25 +1142,26 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>80</v>
+      <c r="A53" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B54" s="6"/>
       <c r="C54" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" t="s">
@@ -1166,10 +1170,20 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C56" t="s">
-        <v>59</v>
+      <c r="B57" s="6"/>
+      <c r="C57" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>